<commit_message>
Added schedule text and gantt chart png
</commit_message>
<xml_diff>
--- a/documentation/design_update/figures/gantt_chart.xlsx
+++ b/documentation/design_update/figures/gantt_chart.xlsx
@@ -154,7 +154,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="m/d;@"/>
+    <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -311,12 +311,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -333,15 +327,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -625,7 +625,7 @@
   <dimension ref="A1:AG34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,919 +665,919 @@
       <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="8">
+      <c r="C1" s="27">
         <v>1</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="8">
+      <c r="D1" s="28"/>
+      <c r="E1" s="27">
         <v>2</v>
       </c>
-      <c r="F1" s="9"/>
-      <c r="G1" s="8">
+      <c r="F1" s="28"/>
+      <c r="G1" s="27">
         <v>3</v>
       </c>
-      <c r="H1" s="9"/>
-      <c r="I1" s="8">
+      <c r="H1" s="28"/>
+      <c r="I1" s="27">
         <v>4</v>
       </c>
-      <c r="J1" s="9"/>
-      <c r="K1" s="8">
+      <c r="J1" s="28"/>
+      <c r="K1" s="27">
         <v>5</v>
       </c>
-      <c r="L1" s="9"/>
-      <c r="M1" s="8">
+      <c r="L1" s="28"/>
+      <c r="M1" s="27">
         <v>6</v>
       </c>
-      <c r="N1" s="9"/>
-      <c r="O1" s="8">
+      <c r="N1" s="28"/>
+      <c r="O1" s="27">
         <v>7</v>
       </c>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="8">
+      <c r="P1" s="28"/>
+      <c r="Q1" s="27">
         <v>8</v>
       </c>
-      <c r="R1" s="9"/>
-      <c r="S1" s="8">
+      <c r="R1" s="28"/>
+      <c r="S1" s="27">
         <v>9</v>
       </c>
-      <c r="T1" s="9"/>
-      <c r="U1" s="8">
+      <c r="T1" s="28"/>
+      <c r="U1" s="27">
         <v>10</v>
       </c>
-      <c r="V1" s="9"/>
-      <c r="W1" s="8">
+      <c r="V1" s="28"/>
+      <c r="W1" s="27">
         <v>11</v>
       </c>
-      <c r="X1" s="9"/>
-      <c r="Y1" s="8">
+      <c r="X1" s="28"/>
+      <c r="Y1" s="27">
         <v>12</v>
       </c>
-      <c r="Z1" s="9"/>
-      <c r="AA1" s="8">
+      <c r="Z1" s="28"/>
+      <c r="AA1" s="27">
         <v>13</v>
       </c>
-      <c r="AB1" s="9"/>
+      <c r="AB1" s="28"/>
       <c r="AC1" s="2"/>
       <c r="AD1" s="3"/>
       <c r="AE1" s="3"/>
       <c r="AF1" s="3"/>
       <c r="AG1" s="3"/>
     </row>
-    <row r="2" spans="1:33" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="24">
+      <c r="C2" s="25">
         <v>42765</v>
       </c>
-      <c r="D2" s="25"/>
-      <c r="E2" s="24">
+      <c r="D2" s="26"/>
+      <c r="E2" s="25">
         <v>42772</v>
       </c>
-      <c r="F2" s="25"/>
-      <c r="G2" s="24">
+      <c r="F2" s="26"/>
+      <c r="G2" s="25">
         <v>42779</v>
       </c>
-      <c r="H2" s="25"/>
-      <c r="I2" s="24">
+      <c r="H2" s="26"/>
+      <c r="I2" s="25">
         <v>42786</v>
       </c>
-      <c r="J2" s="25"/>
-      <c r="K2" s="24">
+      <c r="J2" s="26"/>
+      <c r="K2" s="25">
         <v>42793</v>
       </c>
-      <c r="L2" s="25"/>
-      <c r="M2" s="24">
+      <c r="L2" s="26"/>
+      <c r="M2" s="25">
         <v>42800</v>
       </c>
-      <c r="N2" s="25"/>
-      <c r="O2" s="24">
+      <c r="N2" s="26"/>
+      <c r="O2" s="25">
         <v>42814</v>
       </c>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="24">
+      <c r="P2" s="26"/>
+      <c r="Q2" s="25">
         <v>42821</v>
       </c>
-      <c r="R2" s="25"/>
-      <c r="S2" s="24">
+      <c r="R2" s="26"/>
+      <c r="S2" s="25">
         <v>42828</v>
       </c>
-      <c r="T2" s="25"/>
-      <c r="U2" s="24">
+      <c r="T2" s="26"/>
+      <c r="U2" s="25">
         <v>42835</v>
       </c>
-      <c r="V2" s="25"/>
-      <c r="W2" s="24">
+      <c r="V2" s="26"/>
+      <c r="W2" s="25">
         <v>42841</v>
       </c>
-      <c r="X2" s="25"/>
-      <c r="Y2" s="24">
+      <c r="X2" s="26"/>
+      <c r="Y2" s="25">
         <v>42849</v>
       </c>
-      <c r="Z2" s="25"/>
-      <c r="AA2" s="24">
+      <c r="Z2" s="26"/>
+      <c r="AA2" s="25">
         <v>42856</v>
       </c>
-      <c r="AB2" s="25"/>
+      <c r="AB2" s="26"/>
       <c r="AC2" s="2"/>
       <c r="AD2" s="3"/>
       <c r="AE2" s="3"/>
       <c r="AF2" s="3"/>
       <c r="AG2" s="3"/>
     </row>
-    <row r="3" spans="1:33" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15">
+    <row r="3" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="20"/>
-      <c r="P3" s="21"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="12"/>
-      <c r="T3" s="13"/>
-      <c r="U3" s="12"/>
-      <c r="V3" s="13"/>
-      <c r="W3" s="12"/>
-      <c r="X3" s="13"/>
-      <c r="Y3" s="12"/>
-      <c r="Z3" s="13"/>
-      <c r="AA3" s="12"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="11"/>
+      <c r="W3" s="10"/>
+      <c r="X3" s="11"/>
+      <c r="Y3" s="10"/>
+      <c r="Z3" s="11"/>
+      <c r="AA3" s="10"/>
       <c r="AC3" s="2"/>
       <c r="AD3" s="3"/>
       <c r="AE3" s="3"/>
       <c r="AF3" s="3"/>
       <c r="AG3" s="3"/>
     </row>
-    <row r="4" spans="1:33" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+    <row r="4" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="13"/>
-      <c r="S4" s="12"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="12"/>
-      <c r="V4" s="13"/>
-      <c r="W4" s="12"/>
-      <c r="X4" s="13"/>
-      <c r="Y4" s="12"/>
-      <c r="Z4" s="13"/>
-      <c r="AA4" s="12"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="11"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="11"/>
+      <c r="W4" s="10"/>
+      <c r="X4" s="11"/>
+      <c r="Y4" s="10"/>
+      <c r="Z4" s="11"/>
+      <c r="AA4" s="10"/>
       <c r="AC4" s="2"/>
       <c r="AD4" s="3"/>
       <c r="AE4" s="3"/>
       <c r="AF4" s="3"/>
       <c r="AG4" s="3"/>
     </row>
-    <row r="5" spans="1:33" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+    <row r="5" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="12"/>
-      <c r="R5" s="13"/>
-      <c r="S5" s="12"/>
-      <c r="T5" s="13"/>
-      <c r="U5" s="12"/>
-      <c r="V5" s="13"/>
-      <c r="W5" s="12"/>
-      <c r="X5" s="13"/>
-      <c r="Y5" s="12"/>
-      <c r="Z5" s="13"/>
-      <c r="AA5" s="12"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="11"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="11"/>
+      <c r="W5" s="10"/>
+      <c r="X5" s="11"/>
+      <c r="Y5" s="10"/>
+      <c r="Z5" s="11"/>
+      <c r="AA5" s="10"/>
       <c r="AC5" s="2"/>
       <c r="AD5" s="3"/>
       <c r="AE5" s="3"/>
       <c r="AF5" s="3"/>
       <c r="AG5" s="3"/>
     </row>
-    <row r="6" spans="1:33" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+    <row r="6" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="12"/>
-      <c r="R6" s="13"/>
-      <c r="S6" s="12"/>
-      <c r="T6" s="13"/>
-      <c r="U6" s="12"/>
-      <c r="V6" s="13"/>
-      <c r="W6" s="12"/>
-      <c r="X6" s="13"/>
-      <c r="Y6" s="12"/>
-      <c r="Z6" s="13"/>
-      <c r="AA6" s="12"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="11"/>
+      <c r="W6" s="10"/>
+      <c r="X6" s="11"/>
+      <c r="Y6" s="10"/>
+      <c r="Z6" s="11"/>
+      <c r="AA6" s="10"/>
       <c r="AC6" s="2"/>
       <c r="AD6" s="3"/>
       <c r="AE6" s="3"/>
       <c r="AF6" s="3"/>
       <c r="AG6" s="3"/>
     </row>
-    <row r="7" spans="1:33" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+    <row r="7" spans="1:33" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="12"/>
-      <c r="R7" s="13"/>
-      <c r="S7" s="12"/>
-      <c r="T7" s="13"/>
-      <c r="U7" s="12"/>
-      <c r="V7" s="13"/>
-      <c r="W7" s="12"/>
-      <c r="X7" s="13"/>
-      <c r="Y7" s="12"/>
-      <c r="Z7" s="13"/>
-      <c r="AA7" s="12"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="11"/>
+      <c r="W7" s="10"/>
+      <c r="X7" s="11"/>
+      <c r="Y7" s="10"/>
+      <c r="Z7" s="11"/>
+      <c r="AA7" s="10"/>
       <c r="AC7" s="2"/>
       <c r="AD7" s="3"/>
       <c r="AE7" s="3"/>
       <c r="AF7" s="3"/>
       <c r="AG7" s="3"/>
     </row>
-    <row r="8" spans="1:33" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+    <row r="8" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="13"/>
-      <c r="Q8" s="12"/>
-      <c r="R8" s="13"/>
-      <c r="S8" s="12"/>
-      <c r="T8" s="13"/>
-      <c r="U8" s="12"/>
-      <c r="V8" s="13"/>
-      <c r="W8" s="12"/>
-      <c r="X8" s="13"/>
-      <c r="Y8" s="12"/>
-      <c r="Z8" s="13"/>
-      <c r="AA8" s="12"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="11"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="11"/>
+      <c r="W8" s="10"/>
+      <c r="X8" s="11"/>
+      <c r="Y8" s="10"/>
+      <c r="Z8" s="11"/>
+      <c r="AA8" s="10"/>
       <c r="AC8" s="2"/>
       <c r="AD8" s="3"/>
       <c r="AE8" s="3"/>
       <c r="AF8" s="3"/>
       <c r="AG8" s="3"/>
     </row>
-    <row r="9" spans="1:33" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+    <row r="9" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="12"/>
-      <c r="R9" s="13"/>
-      <c r="S9" s="12"/>
-      <c r="T9" s="13"/>
-      <c r="U9" s="12"/>
-      <c r="V9" s="13"/>
-      <c r="W9" s="12"/>
-      <c r="X9" s="13"/>
-      <c r="Y9" s="12"/>
-      <c r="Z9" s="13"/>
-      <c r="AA9" s="12"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="11"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="11"/>
+      <c r="U9" s="10"/>
+      <c r="V9" s="11"/>
+      <c r="W9" s="10"/>
+      <c r="X9" s="11"/>
+      <c r="Y9" s="10"/>
+      <c r="Z9" s="11"/>
+      <c r="AA9" s="10"/>
       <c r="AC9" s="2"/>
       <c r="AD9" s="3"/>
       <c r="AE9" s="3"/>
       <c r="AF9" s="3"/>
       <c r="AG9" s="3"/>
     </row>
-    <row r="10" spans="1:33" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+    <row r="10" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="21"/>
-      <c r="O10" s="20"/>
-      <c r="P10" s="21"/>
-      <c r="Q10" s="12"/>
-      <c r="R10" s="13"/>
-      <c r="S10" s="12"/>
-      <c r="T10" s="13"/>
-      <c r="U10" s="12"/>
-      <c r="V10" s="13"/>
-      <c r="W10" s="12"/>
-      <c r="X10" s="13"/>
-      <c r="Y10" s="12"/>
-      <c r="Z10" s="13"/>
-      <c r="AA10" s="12"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="19"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="10"/>
+      <c r="V10" s="11"/>
+      <c r="W10" s="10"/>
+      <c r="X10" s="11"/>
+      <c r="Y10" s="10"/>
+      <c r="Z10" s="11"/>
+      <c r="AA10" s="10"/>
       <c r="AC10" s="2"/>
       <c r="AD10" s="3"/>
       <c r="AE10" s="3"/>
       <c r="AF10" s="3"/>
       <c r="AG10" s="3"/>
     </row>
-    <row r="11" spans="1:33" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="15">
+    <row r="11" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="13">
         <v>1.2</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="18"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="12"/>
-      <c r="R11" s="13"/>
-      <c r="S11" s="12"/>
-      <c r="T11" s="13"/>
-      <c r="U11" s="12"/>
-      <c r="V11" s="13"/>
-      <c r="W11" s="12"/>
-      <c r="X11" s="13"/>
-      <c r="Y11" s="12"/>
-      <c r="Z11" s="13"/>
-      <c r="AA11" s="12"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="11"/>
+      <c r="U11" s="10"/>
+      <c r="V11" s="11"/>
+      <c r="W11" s="10"/>
+      <c r="X11" s="11"/>
+      <c r="Y11" s="10"/>
+      <c r="Z11" s="11"/>
+      <c r="AA11" s="10"/>
       <c r="AC11" s="2"/>
       <c r="AD11" s="3"/>
       <c r="AE11" s="3"/>
       <c r="AF11" s="3"/>
       <c r="AG11" s="3"/>
     </row>
-    <row r="12" spans="1:33" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
+    <row r="12" spans="1:33" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="13"/>
-      <c r="Q12" s="12"/>
-      <c r="R12" s="13"/>
-      <c r="S12" s="12"/>
-      <c r="T12" s="13"/>
-      <c r="U12" s="12"/>
-      <c r="V12" s="13"/>
-      <c r="W12" s="12"/>
-      <c r="X12" s="13"/>
-      <c r="Y12" s="12"/>
-      <c r="Z12" s="13"/>
-      <c r="AA12" s="12"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="11"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="11"/>
+      <c r="U12" s="10"/>
+      <c r="V12" s="11"/>
+      <c r="W12" s="10"/>
+      <c r="X12" s="11"/>
+      <c r="Y12" s="10"/>
+      <c r="Z12" s="11"/>
+      <c r="AA12" s="10"/>
       <c r="AC12" s="2"/>
       <c r="AD12" s="3"/>
       <c r="AE12" s="3"/>
       <c r="AF12" s="3"/>
       <c r="AG12" s="3"/>
     </row>
-    <row r="13" spans="1:33" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
+    <row r="13" spans="1:33" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="19"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="13"/>
-      <c r="Q13" s="12"/>
-      <c r="R13" s="13"/>
-      <c r="S13" s="12"/>
-      <c r="T13" s="13"/>
-      <c r="U13" s="12"/>
-      <c r="V13" s="13"/>
-      <c r="W13" s="12"/>
-      <c r="X13" s="13"/>
-      <c r="Y13" s="12"/>
-      <c r="Z13" s="13"/>
-      <c r="AA13" s="12"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="11"/>
+      <c r="S13" s="10"/>
+      <c r="T13" s="11"/>
+      <c r="U13" s="10"/>
+      <c r="V13" s="11"/>
+      <c r="W13" s="10"/>
+      <c r="X13" s="11"/>
+      <c r="Y13" s="10"/>
+      <c r="Z13" s="11"/>
+      <c r="AA13" s="10"/>
       <c r="AC13" s="2"/>
       <c r="AD13" s="3"/>
       <c r="AE13" s="3"/>
       <c r="AF13" s="3"/>
       <c r="AG13" s="3"/>
     </row>
-    <row r="14" spans="1:33" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
+    <row r="14" spans="1:33" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="13"/>
-      <c r="O14" s="12"/>
-      <c r="P14" s="13"/>
-      <c r="Q14" s="12"/>
-      <c r="R14" s="13"/>
-      <c r="S14" s="12"/>
-      <c r="T14" s="13"/>
-      <c r="U14" s="12"/>
-      <c r="V14" s="13"/>
-      <c r="W14" s="12"/>
-      <c r="X14" s="13"/>
-      <c r="Y14" s="12"/>
-      <c r="Z14" s="13"/>
-      <c r="AA14" s="12"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="10"/>
+      <c r="T14" s="11"/>
+      <c r="U14" s="10"/>
+      <c r="V14" s="11"/>
+      <c r="W14" s="10"/>
+      <c r="X14" s="11"/>
+      <c r="Y14" s="10"/>
+      <c r="Z14" s="11"/>
+      <c r="AA14" s="10"/>
       <c r="AC14" s="2"/>
       <c r="AD14" s="3"/>
       <c r="AE14" s="3"/>
       <c r="AF14" s="3"/>
       <c r="AG14" s="3"/>
     </row>
-    <row r="15" spans="1:33" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
+    <row r="15" spans="1:33" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="18"/>
-      <c r="O15" s="12"/>
-      <c r="P15" s="13"/>
-      <c r="Q15" s="12"/>
-      <c r="R15" s="13"/>
-      <c r="S15" s="12"/>
-      <c r="T15" s="13"/>
-      <c r="U15" s="12"/>
-      <c r="V15" s="13"/>
-      <c r="W15" s="12"/>
-      <c r="X15" s="13"/>
-      <c r="Y15" s="12"/>
-      <c r="Z15" s="13"/>
-      <c r="AA15" s="12"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="10"/>
+      <c r="T15" s="11"/>
+      <c r="U15" s="10"/>
+      <c r="V15" s="11"/>
+      <c r="W15" s="10"/>
+      <c r="X15" s="11"/>
+      <c r="Y15" s="10"/>
+      <c r="Z15" s="11"/>
+      <c r="AA15" s="10"/>
       <c r="AC15" s="2"/>
       <c r="AD15" s="3"/>
       <c r="AE15" s="3"/>
       <c r="AF15" s="3"/>
       <c r="AG15" s="3"/>
     </row>
-    <row r="16" spans="1:33" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
+    <row r="16" spans="1:33" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="12"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="13"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="13"/>
-      <c r="Q16" s="12"/>
-      <c r="R16" s="13"/>
-      <c r="S16" s="12"/>
-      <c r="T16" s="13"/>
-      <c r="U16" s="12"/>
-      <c r="V16" s="13"/>
-      <c r="W16" s="12"/>
-      <c r="X16" s="13"/>
-      <c r="Y16" s="12"/>
-      <c r="Z16" s="13"/>
-      <c r="AA16" s="12"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="11"/>
+      <c r="S16" s="10"/>
+      <c r="T16" s="11"/>
+      <c r="U16" s="10"/>
+      <c r="V16" s="11"/>
+      <c r="W16" s="10"/>
+      <c r="X16" s="11"/>
+      <c r="Y16" s="10"/>
+      <c r="Z16" s="11"/>
+      <c r="AA16" s="10"/>
       <c r="AC16" s="2"/>
       <c r="AD16" s="3"/>
       <c r="AE16" s="3"/>
       <c r="AF16" s="3"/>
       <c r="AG16" s="3"/>
     </row>
-    <row r="17" spans="1:33" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
+    <row r="17" spans="1:33" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="12"/>
-      <c r="P17" s="13"/>
-      <c r="Q17" s="12"/>
-      <c r="R17" s="13"/>
-      <c r="S17" s="12"/>
-      <c r="T17" s="13"/>
-      <c r="U17" s="12"/>
-      <c r="V17" s="13"/>
-      <c r="W17" s="12"/>
-      <c r="X17" s="13"/>
-      <c r="Y17" s="12"/>
-      <c r="Z17" s="13"/>
-      <c r="AA17" s="12"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="11"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="11"/>
+      <c r="U17" s="10"/>
+      <c r="V17" s="11"/>
+      <c r="W17" s="10"/>
+      <c r="X17" s="11"/>
+      <c r="Y17" s="10"/>
+      <c r="Z17" s="11"/>
+      <c r="AA17" s="10"/>
       <c r="AC17" s="2"/>
       <c r="AD17" s="3"/>
       <c r="AE17" s="3"/>
       <c r="AF17" s="3"/>
       <c r="AG17" s="3"/>
     </row>
-    <row r="18" spans="1:33" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
+    <row r="18" spans="1:33" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="12"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="13"/>
-      <c r="O18" s="17"/>
-      <c r="P18" s="18"/>
-      <c r="Q18" s="12"/>
-      <c r="R18" s="13"/>
-      <c r="S18" s="12"/>
-      <c r="T18" s="13"/>
-      <c r="U18" s="12"/>
-      <c r="V18" s="13"/>
-      <c r="W18" s="12"/>
-      <c r="X18" s="13"/>
-      <c r="Y18" s="12"/>
-      <c r="Z18" s="13"/>
-      <c r="AA18" s="12"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="15"/>
+      <c r="P18" s="16"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="11"/>
+      <c r="S18" s="10"/>
+      <c r="T18" s="11"/>
+      <c r="U18" s="10"/>
+      <c r="V18" s="11"/>
+      <c r="W18" s="10"/>
+      <c r="X18" s="11"/>
+      <c r="Y18" s="10"/>
+      <c r="Z18" s="11"/>
+      <c r="AA18" s="10"/>
       <c r="AC18" s="2"/>
       <c r="AD18" s="3"/>
       <c r="AE18" s="3"/>
       <c r="AF18" s="3"/>
       <c r="AG18" s="3"/>
     </row>
-    <row r="19" spans="1:33" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="15">
+    <row r="19" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="13">
         <v>1.3</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="12"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="12"/>
-      <c r="P19" s="13"/>
-      <c r="Q19" s="14"/>
-      <c r="R19" s="16"/>
-      <c r="S19" s="14"/>
-      <c r="T19" s="16"/>
-      <c r="U19" s="14"/>
-      <c r="V19" s="16"/>
-      <c r="W19" s="14"/>
-      <c r="X19" s="16"/>
-      <c r="Y19" s="14"/>
-      <c r="Z19" s="16"/>
-      <c r="AA19" s="14"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="14"/>
+      <c r="S19" s="12"/>
+      <c r="T19" s="14"/>
+      <c r="U19" s="12"/>
+      <c r="V19" s="14"/>
+      <c r="W19" s="12"/>
+      <c r="X19" s="14"/>
+      <c r="Y19" s="12"/>
+      <c r="Z19" s="14"/>
+      <c r="AA19" s="12"/>
       <c r="AC19" s="2"/>
       <c r="AD19" s="3"/>
       <c r="AE19" s="3"/>
       <c r="AF19" s="3"/>
       <c r="AG19" s="3"/>
     </row>
-    <row r="20" spans="1:33" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
+    <row r="20" spans="1:33" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="12"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="12"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="12"/>
-      <c r="P20" s="13"/>
-      <c r="Q20" s="14"/>
-      <c r="R20" s="16"/>
-      <c r="S20" s="12"/>
-      <c r="T20" s="13"/>
-      <c r="U20" s="12"/>
-      <c r="V20" s="13"/>
-      <c r="W20" s="12"/>
-      <c r="X20" s="13"/>
-      <c r="Y20" s="12"/>
-      <c r="Z20" s="13"/>
-      <c r="AA20" s="12"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="14"/>
+      <c r="S20" s="10"/>
+      <c r="T20" s="11"/>
+      <c r="U20" s="10"/>
+      <c r="V20" s="11"/>
+      <c r="W20" s="10"/>
+      <c r="X20" s="11"/>
+      <c r="Y20" s="10"/>
+      <c r="Z20" s="11"/>
+      <c r="AA20" s="10"/>
       <c r="AC20" s="2"/>
       <c r="AD20" s="3"/>
       <c r="AE20" s="3"/>
       <c r="AF20" s="3"/>
       <c r="AG20" s="3"/>
     </row>
-    <row r="21" spans="1:33" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
+    <row r="21" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="12"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="12"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="12"/>
-      <c r="P21" s="13"/>
-      <c r="Q21" s="12"/>
-      <c r="R21" s="13"/>
-      <c r="S21" s="14"/>
-      <c r="T21" s="16"/>
-      <c r="U21" s="14"/>
-      <c r="V21" s="16"/>
-      <c r="W21" s="14"/>
-      <c r="X21" s="16"/>
-      <c r="Y21" s="12"/>
-      <c r="Z21" s="13"/>
-      <c r="AA21" s="12"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="11"/>
+      <c r="S21" s="12"/>
+      <c r="T21" s="14"/>
+      <c r="U21" s="12"/>
+      <c r="V21" s="14"/>
+      <c r="W21" s="12"/>
+      <c r="X21" s="14"/>
+      <c r="Y21" s="10"/>
+      <c r="Z21" s="11"/>
+      <c r="AA21" s="10"/>
       <c r="AC21" s="2"/>
       <c r="AD21" s="3"/>
       <c r="AE21" s="3"/>
       <c r="AF21" s="3"/>
       <c r="AG21" s="3"/>
     </row>
-    <row r="22" spans="1:33" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
+    <row r="22" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="12"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="12"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="12"/>
-      <c r="P22" s="13"/>
-      <c r="Q22" s="12"/>
-      <c r="R22" s="13"/>
-      <c r="S22" s="12"/>
-      <c r="T22" s="13"/>
-      <c r="U22" s="12"/>
-      <c r="V22" s="13"/>
-      <c r="W22" s="12"/>
-      <c r="X22" s="13"/>
-      <c r="Y22" s="14"/>
-      <c r="Z22" s="16"/>
-      <c r="AA22" s="12"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="11"/>
+      <c r="S22" s="10"/>
+      <c r="T22" s="11"/>
+      <c r="U22" s="10"/>
+      <c r="V22" s="11"/>
+      <c r="W22" s="10"/>
+      <c r="X22" s="11"/>
+      <c r="Y22" s="12"/>
+      <c r="Z22" s="14"/>
+      <c r="AA22" s="10"/>
       <c r="AC22" s="2"/>
       <c r="AD22" s="3"/>
       <c r="AE22" s="3"/>
       <c r="AF22" s="3"/>
       <c r="AG22" s="3"/>
     </row>
-    <row r="23" spans="1:33" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="26"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="27"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="27"/>
-      <c r="K23" s="26"/>
-      <c r="L23" s="27"/>
-      <c r="M23" s="26"/>
-      <c r="N23" s="27"/>
-      <c r="O23" s="26"/>
-      <c r="P23" s="27"/>
-      <c r="Q23" s="26"/>
-      <c r="R23" s="27"/>
-      <c r="S23" s="26"/>
-      <c r="T23" s="27"/>
-      <c r="U23" s="26"/>
-      <c r="V23" s="27"/>
-      <c r="W23" s="26"/>
-      <c r="X23" s="27"/>
-      <c r="Y23" s="26"/>
-      <c r="Z23" s="27"/>
-      <c r="AA23" s="28"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="22"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="22"/>
+      <c r="N23" s="23"/>
+      <c r="O23" s="22"/>
+      <c r="P23" s="23"/>
+      <c r="Q23" s="22"/>
+      <c r="R23" s="23"/>
+      <c r="S23" s="22"/>
+      <c r="T23" s="23"/>
+      <c r="U23" s="22"/>
+      <c r="V23" s="23"/>
+      <c r="W23" s="22"/>
+      <c r="X23" s="23"/>
+      <c r="Y23" s="22"/>
+      <c r="Z23" s="23"/>
+      <c r="AA23" s="24"/>
       <c r="AB23" s="6"/>
       <c r="AC23" s="2"/>
       <c r="AD23" s="3"/>
@@ -1918,19 +1918,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="AA2:AB2"/>
-    <mergeCell ref="U1:V1"/>
-    <mergeCell ref="W1:X1"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="AA1:AB1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="Q1:R1"/>
     <mergeCell ref="S1:T1"/>
@@ -1944,6 +1931,19 @@
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="M1:N1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="AA2:AB2"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="AA1:AB1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>